<commit_message>
Replaced missing conditional formatting in the HEM/BC results template
</commit_message>
<xml_diff>
--- a/src/class_HEMBC/results_template.xlsx
+++ b/src/class_HEMBC/results_template.xlsx
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -74,7 +70,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -392,55 +409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>G1&lt;&gt;F1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>$B1=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
-      <formula>$C1=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,4 +449,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="I1 G1:G1048576 I3:I1048576">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>G1&lt;&gt;F1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>I2&lt;&gt;H2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>$C1=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>